<commit_message>
update data dictionary and add arcade code
</commit_message>
<xml_diff>
--- a/raw_data/SCBI_data_dictionary_2023_census.xlsx
+++ b/raw_data/SCBI_data_dictionary_2023_census.xlsx
@@ -5,48 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\shuej\Dropbox (Smithsonian)\Field_Form_Data_Entry\SCBI\census_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/shuej_si_edu/Documents/Documents/GitHub/2023census/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C450C2-E468-42CE-BFDB-408AA2E9E744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C407AD3B-5D82-4C4B-A740-7178B27B56FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="existing_trees" sheetId="1" r:id="rId1"/>
     <sheet name="existing_stems" sheetId="3" r:id="rId2"/>
     <sheet name="mortality_fields" sheetId="4" r:id="rId3"/>
-    <sheet name="recruits" sheetId="2" r:id="rId4"/>
-    <sheet name="personnel" sheetId="8" r:id="rId5"/>
-    <sheet name="code_choices" sheetId="5" r:id="rId6"/>
+    <sheet name="code_choices" sheetId="5" r:id="rId4"/>
+    <sheet name="recruits" sheetId="2" r:id="rId5"/>
+    <sheet name="personnel" sheetId="8" r:id="rId6"/>
     <sheet name="status_2023" sheetId="7" r:id="rId7"/>
     <sheet name="census_status" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">existing_trees!$B$1:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">existing_trees!$B$1:$G$36</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="263">
   <si>
     <t>crown_position</t>
   </si>
@@ -405,9 +394,6 @@
     <t>A, AU</t>
   </si>
   <si>
-    <t>denotes whether a tree is multistemmed; use to create mutlistem view</t>
-  </si>
-  <si>
     <t>hide (0 - don't collect mortality data) or show (1 - collect mortality data) the following fields</t>
   </si>
   <si>
@@ -549,9 +535,6 @@
     <t>Rachel Hoffman</t>
   </si>
   <si>
-    <t>RF</t>
-  </si>
-  <si>
     <t>not started</t>
   </si>
   <si>
@@ -636,9 +619,6 @@
     <t>tree_dead</t>
   </si>
   <si>
-    <t>DBH_check</t>
-  </si>
-  <si>
     <t>DBH check</t>
   </si>
   <si>
@@ -649,6 +629,201 @@
   </si>
   <si>
     <t>crown_living</t>
+  </si>
+  <si>
+    <t>previous_codes</t>
+  </si>
+  <si>
+    <t>previous_dbh</t>
+  </si>
+  <si>
+    <t>mortality_status</t>
+  </si>
+  <si>
+    <t>mort_comment</t>
+  </si>
+  <si>
+    <t>previous_status</t>
+  </si>
+  <si>
+    <t>0,1,2,3</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>0 - tree is alive; 1 - entire tree is dead</t>
+  </si>
+  <si>
+    <t>dbh_currentCensus</t>
+  </si>
+  <si>
+    <t>status_currentCensus</t>
+  </si>
+  <si>
+    <t>codes_currentCensus</t>
+  </si>
+  <si>
+    <t>notes_currentCensus</t>
+  </si>
+  <si>
+    <t>dbh_check</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Alive unhealthy</t>
+  </si>
+  <si>
+    <t>Alive</t>
+  </si>
+  <si>
+    <t>No direct light; only receives filtered light through other trees</t>
+  </si>
+  <si>
+    <t>Lateral light; &lt;10% exposed to vertical light</t>
+  </si>
+  <si>
+    <t>Some overhead light</t>
+  </si>
+  <si>
+    <t>Full overhead light; &gt;90% exposed to vertical light</t>
+  </si>
+  <si>
+    <t>Canopy completely exposed to overhead and lateral light</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Unable to determine</t>
+  </si>
+  <si>
+    <t>Broken stem</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>Crushed by other tree</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Uprooted tree</t>
+  </si>
+  <si>
+    <t>Slope failure</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>Animal damage</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Bark beetles (not including EAB)</t>
+  </si>
+  <si>
+    <t>Insect infection (including EAB)</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>Complete defoliation for a portion of stem</t>
+  </si>
+  <si>
+    <t>Fungi visible</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Canker or swelling</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Leaf damage</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Wound</t>
+  </si>
+  <si>
+    <t>Rotting stem</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Root damage</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Armillaria root disease</t>
+  </si>
+  <si>
+    <t>lianas absent from tree crown</t>
+  </si>
+  <si>
+    <t>up to 25% of tree crown covered by lianas</t>
+  </si>
+  <si>
+    <t>26-50% liana cover</t>
+  </si>
+  <si>
+    <t>51-75% liana cover</t>
+  </si>
+  <si>
+    <t>76-100% liana cover</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>massive</t>
+  </si>
+  <si>
+    <t>crown_check</t>
+  </si>
+  <si>
+    <t>to populate error if crown_intact &lt; crown_living</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>dbh_mm_currentCensus</t>
+  </si>
+  <si>
+    <t>denotes whether a tree is multistemmed; calculated currently as field was incorrect</t>
   </si>
 </sst>
 </file>
@@ -707,17 +882,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1034,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CAB06-B581-49AF-A77A-B8530B1E5C50}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1220,7 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1081,7 +1252,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1095,37 +1266,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1148,7 +1318,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1168,7 +1338,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1191,7 +1361,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1205,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1219,11 +1389,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
@@ -1233,233 +1406,483 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>198</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
       <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="C17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" s="6">
-        <v>5</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17"/>
       <c r="F17" t="b">
         <v>0</v>
       </c>
-      <c r="G17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="B18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="4">
+        <v>5</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
         <v>171</v>
       </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="C20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>132</v>
+      </c>
+      <c r="K28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30"/>
+      <c r="G30" t="s">
         <v>195</v>
       </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>261</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1470,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3688775-B1D1-40DD-BD64-506E041BD460}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,10 +1936,10 @@
         <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,30 +1961,29 @@
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" t="s">
         <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1644,6 +2066,9 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
@@ -1654,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1668,7 +2093,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1679,6 +2104,9 @@
         <v>52</v>
       </c>
       <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -1697,6 +2125,9 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
       </c>
       <c r="D11" t="s">
@@ -1715,6 +2146,9 @@
         <v>52</v>
       </c>
       <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
         <v>63</v>
       </c>
       <c r="D12" t="s">
@@ -1736,6 +2170,9 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" t="s">
         <v>66</v>
       </c>
       <c r="D13" t="s">
@@ -1766,63 +2203,66 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="F15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="4">
         <v>5</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="4">
         <v>0</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I16" t="s">
         <v>72</v>
@@ -1836,7 +2276,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -1862,6 +2302,9 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" t="s">
         <v>28</v>
       </c>
       <c r="D18" t="s">
@@ -1872,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K18" t="s">
         <v>73</v>
@@ -1883,7 +2326,7 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -1893,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K19" t="s">
         <v>73</v>
@@ -1904,6 +2347,9 @@
         <v>52</v>
       </c>
       <c r="B20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
@@ -1925,7 +2371,7 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1934,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1942,24 +2388,35 @@
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>184</v>
+      <c r="B23" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1969,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9274B4-E0C8-460A-8E93-CD49FCA1D6B5}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,7 +2469,7 @@
         <v>69</v>
       </c>
       <c r="J1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2029,7 +2486,7 @@
         <v>118</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" t="s">
         <v>101</v>
@@ -2046,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -2069,10 +2526,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -2095,10 +2552,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
@@ -2113,7 +2570,7 @@
         <v>114</v>
       </c>
       <c r="J5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2130,13 +2587,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" t="s">
         <v>115</v>
-      </c>
-      <c r="I6">
-        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2144,16 +2598,16 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>141</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>142</v>
       </c>
       <c r="H7" t="s">
         <v>115</v>
@@ -2167,7 +2621,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
@@ -2190,7 +2644,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -2213,7 +2667,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -2236,7 +2690,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
@@ -2262,7 +2716,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -2271,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" t="s">
         <v>114</v>
@@ -2285,7 +2739,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -2298,6 +2752,23 @@
       </c>
       <c r="H13" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2306,10 +2777,711 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550619-C900-43DA-89F1-CA09A5AF18CE}">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>233</v>
+      </c>
+      <c r="C37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" t="s">
+        <v>246</v>
+      </c>
+      <c r="C45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4152C55-78A6-4160-9CEB-224E8F4069AF}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2342,7 +3514,7 @@
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2559,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2601,13 +3773,13 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
         <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2881,12 +4053,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D53756-B6B7-49BD-874B-0633AEB134B2}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,74 +4068,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
         <v>150</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
         <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
         <v>164</v>
-      </c>
-      <c r="B3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
         <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
         <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
         <v>152</v>
-      </c>
-      <c r="B8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
         <v>160</v>
-      </c>
-      <c r="B9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2978,184 +4150,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
     <sortCondition ref="A3:A11"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550619-C900-43DA-89F1-CA09A5AF18CE}">
-  <dimension ref="A1:B20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3244,7 +4238,7 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3252,10 +4246,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3263,10 +4257,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3274,10 +4268,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3285,10 +4279,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consolidating data dictionary with new code list (and deleting other file)
@jess-shue, FYI
</commit_message>
<xml_diff>
--- a/raw_data/SCBI_data_dictionary_2023_census.xlsx
+++ b/raw_data/SCBI_data_dictionary_2023_census.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/shuej_si_edu/Documents/Documents/GitHub/2023census/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herrmannV\Dropbox (Smithsonian)\GitHub\SCBI-ForestGEO\2023census\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C407AD3B-5D82-4C4B-A740-7178B27B56FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25194A6-885B-4C01-9988-5DD7DA592AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="existing_trees" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="270">
   <si>
     <t>crown_position</t>
   </si>
@@ -301,18 +301,12 @@
     <t>within deer exclosure</t>
   </si>
   <si>
-    <t>ID to Genus uncertain</t>
-  </si>
-  <si>
     <t>stem irregular where measured</t>
   </si>
   <si>
     <t>stem bent</t>
   </si>
   <si>
-    <t>stem leaning</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>RT</t>
   </si>
   <si>
-    <t>NN</t>
-  </si>
-  <si>
     <t>multiple stems</t>
   </si>
   <si>
@@ -337,9 +328,6 @@
     <t>replace tag</t>
   </si>
   <si>
-    <t>new nail or wire</t>
-  </si>
-  <si>
     <t>LI</t>
   </si>
   <si>
@@ -424,9 +412,6 @@
     <t>stem broken below 1.3m</t>
   </si>
   <si>
-    <t>resprout</t>
-  </si>
-  <si>
     <t>code_choices</t>
   </si>
   <si>
@@ -595,9 +580,6 @@
     <t>NEEDED for SURVEY123 connection</t>
   </si>
   <si>
-    <t>stem prostrate</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -824,13 +806,52 @@
   </si>
   <si>
     <t>denotes whether a tree is multistemmed; calculated currently as field was incorrect</t>
+  </si>
+  <si>
+    <t>code_pre2023</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>on live stem</t>
+  </si>
+  <si>
+    <t>ID to Genus certain</t>
+  </si>
+  <si>
+    <t>stem leaning - 45 degrees or greater</t>
+  </si>
+  <si>
+    <t>applies to main/largest stem with a secondary stem; also when a secondary stem has a measurable stem</t>
+  </si>
+  <si>
+    <t>stem prostrate - parallel to the ground/on the ground</t>
+  </si>
+  <si>
+    <t>stem dead; living reprouts or epicormic branches below 1.3m</t>
+  </si>
+  <si>
+    <t>not used for stem with status LI</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>DBH verified</t>
+  </si>
+  <si>
+    <t>live or dead - any time the DBH check note appears, but measurement is confirmed</t>
+  </si>
+  <si>
+    <t>no longer used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +863,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -882,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -891,6 +919,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,20 +1237,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CAB06-B581-49AF-A77A-B8530B1E5C50}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1252,7 +1282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1266,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1292,10 +1322,10 @@
         <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1318,7 +1348,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1368,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1361,7 +1391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1389,12 +1419,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1406,13 +1436,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1426,12 +1456,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1446,12 +1476,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -1463,7 +1493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1483,7 +1513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1503,12 +1533,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
@@ -1523,12 +1553,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
         <v>66</v>
@@ -1540,15 +1570,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -1563,33 +1593,33 @@
         <v>5</v>
       </c>
       <c r="J17" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -1603,13 +1633,13 @@
         <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H19" s="4">
         <v>5</v>
@@ -1621,15 +1651,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
@@ -1639,18 +1669,18 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1660,18 +1690,18 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
@@ -1681,18 +1711,18 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
@@ -1702,18 +1732,18 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
@@ -1728,15 +1758,15 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
@@ -1745,13 +1775,13 @@
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I25" t="s">
         <v>72</v>
@@ -1760,12 +1790,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
@@ -1787,12 +1817,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1804,18 +1834,18 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
@@ -1824,18 +1854,18 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
@@ -1853,36 +1883,36 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
         <v>23</v>
       </c>
       <c r="E30"/>
       <c r="G30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D31" t="s">
         <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1895,19 +1925,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3688775-B1D1-40DD-BD64-506E041BD460}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1936,13 +1966,13 @@
         <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1957,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1983,10 +2013,10 @@
         <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2010,7 +2040,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2031,7 +2061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2046,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2061,12 +2091,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -2079,10 +2109,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2093,18 +2123,18 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -2120,12 +2150,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -2141,12 +2171,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
         <v>63</v>
@@ -2165,12 +2195,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
@@ -2186,7 +2216,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2203,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2223,13 +2253,13 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -2242,12 +2272,12 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -2256,13 +2286,13 @@
         <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
         <v>72</v>
@@ -2271,12 +2301,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -2297,12 +2327,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -2315,18 +2345,18 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -2336,18 +2366,18 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -2366,12 +2396,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -2380,40 +2410,40 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
@@ -2429,18 +2459,19 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -2463,39 +2494,39 @@
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I1" t="s">
         <v>69</v>
       </c>
       <c r="J1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2503,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -2515,10 +2546,10 @@
         <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2526,10 +2557,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -2541,10 +2572,10 @@
         <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2552,10 +2583,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
@@ -2567,13 +2598,13 @@
         <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2587,18 +2618,18 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -2607,13 +2638,13 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2621,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
@@ -2633,10 +2664,10 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2644,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -2656,10 +2687,10 @@
         <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2667,7 +2698,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -2679,10 +2710,10 @@
         <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2690,7 +2721,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
@@ -2702,10 +2733,10 @@
         <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2716,7 +2747,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -2725,13 +2756,13 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2739,7 +2770,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -2751,15 +2782,15 @@
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -2768,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2778,21 +2809,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550619-C900-43DA-89F1-CA09A5AF18CE}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
         <v>74</v>
@@ -2800,10 +2832,16 @@
       <c r="C1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -2812,9 +2850,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -2822,217 +2860,254 @@
       <c r="C3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3040,10 +3115,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3051,10 +3126,10 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3062,10 +3137,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -3073,10 +3148,10 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3084,12 +3159,12 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
         <v>76</v>
@@ -3098,205 +3173,205 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
       </c>
       <c r="C34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>225</v>
+      </c>
+      <c r="C36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" t="s">
-        <v>229</v>
-      </c>
-      <c r="C35" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" t="s">
-        <v>231</v>
-      </c>
-      <c r="C36" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>140</v>
-      </c>
-      <c r="B37" t="s">
-        <v>233</v>
-      </c>
-      <c r="C37" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" t="s">
         <v>239</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>140</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C45" t="s">
         <v>241</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C46" t="s">
         <v>243</v>
       </c>
-      <c r="C43" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" t="s">
-        <v>246</v>
-      </c>
-      <c r="C45" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" t="s">
-        <v>248</v>
-      </c>
-      <c r="C46" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -3304,10 +3379,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -3315,10 +3390,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3326,10 +3401,10 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -3337,10 +3412,10 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3348,10 +3423,10 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3359,10 +3434,10 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -3370,10 +3445,10 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -3381,10 +3456,10 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -3392,10 +3467,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -3403,10 +3478,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -3414,10 +3489,10 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -3425,10 +3500,10 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -3436,10 +3511,10 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -3447,10 +3522,10 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -3461,7 +3536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -3485,13 +3560,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3514,10 +3589,10 @@
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3531,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3548,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3562,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -3576,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3590,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -3607,7 +3682,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -3624,7 +3699,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3641,7 +3716,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -3658,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -3679,7 +3754,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3696,7 +3771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -3713,7 +3788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3731,10 +3806,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3751,7 +3826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -3768,21 +3843,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3800,7 +3875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -3821,7 +3896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -3842,7 +3917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -3863,7 +3938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -3882,7 +3957,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -3903,7 +3978,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -3924,7 +3999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3945,7 +4020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
@@ -3966,7 +4041,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -3987,7 +4062,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -4008,7 +4083,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -4029,7 +4104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
@@ -4061,84 +4136,84 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
         <v>149</v>
       </c>
-      <c r="B1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
         <v>155</v>
       </c>
-      <c r="B2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -4162,9 +4237,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4172,44 +4247,44 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4225,12 +4300,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4238,51 +4313,51 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consolidating data dictionary with new code list (and deleting other file) #22
@jess-shue, FYI
</commit_message>
<xml_diff>
--- a/raw_data/SCBI_data_dictionary_2023_census.xlsx
+++ b/raw_data/SCBI_data_dictionary_2023_census.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/shuej_si_edu/Documents/Documents/GitHub/2023census/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herrmannV\Dropbox (Smithsonian)\GitHub\SCBI-ForestGEO\2023census\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C407AD3B-5D82-4C4B-A740-7178B27B56FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25194A6-885B-4C01-9988-5DD7DA592AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="existing_trees" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="270">
   <si>
     <t>crown_position</t>
   </si>
@@ -301,18 +301,12 @@
     <t>within deer exclosure</t>
   </si>
   <si>
-    <t>ID to Genus uncertain</t>
-  </si>
-  <si>
     <t>stem irregular where measured</t>
   </si>
   <si>
     <t>stem bent</t>
   </si>
   <si>
-    <t>stem leaning</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>RT</t>
   </si>
   <si>
-    <t>NN</t>
-  </si>
-  <si>
     <t>multiple stems</t>
   </si>
   <si>
@@ -337,9 +328,6 @@
     <t>replace tag</t>
   </si>
   <si>
-    <t>new nail or wire</t>
-  </si>
-  <si>
     <t>LI</t>
   </si>
   <si>
@@ -424,9 +412,6 @@
     <t>stem broken below 1.3m</t>
   </si>
   <si>
-    <t>resprout</t>
-  </si>
-  <si>
     <t>code_choices</t>
   </si>
   <si>
@@ -595,9 +580,6 @@
     <t>NEEDED for SURVEY123 connection</t>
   </si>
   <si>
-    <t>stem prostrate</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -824,13 +806,52 @@
   </si>
   <si>
     <t>denotes whether a tree is multistemmed; calculated currently as field was incorrect</t>
+  </si>
+  <si>
+    <t>code_pre2023</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>on live stem</t>
+  </si>
+  <si>
+    <t>ID to Genus certain</t>
+  </si>
+  <si>
+    <t>stem leaning - 45 degrees or greater</t>
+  </si>
+  <si>
+    <t>applies to main/largest stem with a secondary stem; also when a secondary stem has a measurable stem</t>
+  </si>
+  <si>
+    <t>stem prostrate - parallel to the ground/on the ground</t>
+  </si>
+  <si>
+    <t>stem dead; living reprouts or epicormic branches below 1.3m</t>
+  </si>
+  <si>
+    <t>not used for stem with status LI</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>DBH verified</t>
+  </si>
+  <si>
+    <t>live or dead - any time the DBH check note appears, but measurement is confirmed</t>
+  </si>
+  <si>
+    <t>no longer used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +863,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -882,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -891,6 +919,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,20 +1237,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CAB06-B581-49AF-A77A-B8530B1E5C50}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1252,7 +1282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1266,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1292,10 +1322,10 @@
         <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1318,7 +1348,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1368,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1361,7 +1391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1389,12 +1419,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1406,13 +1436,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1426,12 +1456,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1446,12 +1476,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -1463,7 +1493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1483,7 +1513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1503,12 +1533,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
@@ -1523,12 +1553,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
         <v>66</v>
@@ -1540,15 +1570,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -1563,33 +1593,33 @@
         <v>5</v>
       </c>
       <c r="J17" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -1603,13 +1633,13 @@
         <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H19" s="4">
         <v>5</v>
@@ -1621,15 +1651,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
@@ -1639,18 +1669,18 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1660,18 +1690,18 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
@@ -1681,18 +1711,18 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
@@ -1702,18 +1732,18 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
@@ -1728,15 +1758,15 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
@@ -1745,13 +1775,13 @@
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I25" t="s">
         <v>72</v>
@@ -1760,12 +1790,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
@@ -1787,12 +1817,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1804,18 +1834,18 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
@@ -1824,18 +1854,18 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
@@ -1853,36 +1883,36 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
         <v>23</v>
       </c>
       <c r="E30"/>
       <c r="G30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D31" t="s">
         <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1895,19 +1925,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3688775-B1D1-40DD-BD64-506E041BD460}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1936,13 +1966,13 @@
         <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1957,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1983,10 +2013,10 @@
         <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2010,7 +2040,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2031,7 +2061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2046,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2061,12 +2091,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -2079,10 +2109,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2093,18 +2123,18 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -2120,12 +2150,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -2141,12 +2171,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
         <v>63</v>
@@ -2165,12 +2195,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
@@ -2186,7 +2216,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2203,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2223,13 +2253,13 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H15" s="4">
         <v>5</v>
@@ -2242,12 +2272,12 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -2256,13 +2286,13 @@
         <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
         <v>72</v>
@@ -2271,12 +2301,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -2297,12 +2327,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -2315,18 +2345,18 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -2336,18 +2366,18 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -2366,12 +2396,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -2380,40 +2410,40 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
@@ -2429,18 +2459,19 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -2463,39 +2494,39 @@
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I1" t="s">
         <v>69</v>
       </c>
       <c r="J1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2503,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -2515,10 +2546,10 @@
         <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2526,10 +2557,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -2541,10 +2572,10 @@
         <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2552,10 +2583,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
@@ -2567,13 +2598,13 @@
         <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2587,18 +2618,18 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -2607,13 +2638,13 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2621,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
@@ -2633,10 +2664,10 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2644,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -2656,10 +2687,10 @@
         <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2667,7 +2698,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -2679,10 +2710,10 @@
         <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2690,7 +2721,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
@@ -2702,10 +2733,10 @@
         <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2716,7 +2747,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -2725,13 +2756,13 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2739,7 +2770,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -2751,15 +2782,15 @@
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -2768,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2778,21 +2809,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550619-C900-43DA-89F1-CA09A5AF18CE}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
         <v>74</v>
@@ -2800,10 +2832,16 @@
       <c r="C1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -2812,9 +2850,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -2822,217 +2860,254 @@
       <c r="C3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3040,10 +3115,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3051,10 +3126,10 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3062,10 +3137,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -3073,10 +3148,10 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3084,12 +3159,12 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
         <v>76</v>
@@ -3098,205 +3173,205 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
       </c>
       <c r="C34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>225</v>
+      </c>
+      <c r="C36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" t="s">
-        <v>229</v>
-      </c>
-      <c r="C35" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" t="s">
-        <v>231</v>
-      </c>
-      <c r="C36" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>140</v>
-      </c>
-      <c r="B37" t="s">
-        <v>233</v>
-      </c>
-      <c r="C37" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
         <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" t="s">
         <v>239</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>140</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C45" t="s">
         <v>241</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C46" t="s">
         <v>243</v>
       </c>
-      <c r="C43" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" t="s">
-        <v>246</v>
-      </c>
-      <c r="C45" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" t="s">
-        <v>248</v>
-      </c>
-      <c r="C46" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -3304,10 +3379,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -3315,10 +3390,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3326,10 +3401,10 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -3337,10 +3412,10 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3348,10 +3423,10 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3359,10 +3434,10 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -3370,10 +3445,10 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -3381,10 +3456,10 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -3392,10 +3467,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -3403,10 +3478,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -3414,10 +3489,10 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -3425,10 +3500,10 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -3436,10 +3511,10 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -3447,10 +3522,10 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -3461,7 +3536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -3485,13 +3560,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3514,10 +3589,10 @@
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3531,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3548,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3562,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -3576,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3590,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -3607,7 +3682,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -3624,7 +3699,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3641,7 +3716,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -3658,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -3679,7 +3754,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3696,7 +3771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -3713,7 +3788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3731,10 +3806,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3751,7 +3826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -3768,21 +3843,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3800,7 +3875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -3821,7 +3896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -3842,7 +3917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -3863,7 +3938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -3882,7 +3957,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -3903,7 +3978,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -3924,7 +3999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3945,7 +4020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
@@ -3966,7 +4041,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -3987,7 +4062,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -4008,7 +4083,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -4029,7 +4104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
@@ -4061,84 +4136,84 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
         <v>149</v>
       </c>
-      <c r="B1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
         <v>155</v>
       </c>
-      <c r="B2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -4162,9 +4237,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4172,44 +4247,44 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4225,12 +4300,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4238,51 +4313,51 @@
         <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data dictionary and arcade code
</commit_message>
<xml_diff>
--- a/raw_data/SCBI_data_dictionary_2023_census.xlsx
+++ b/raw_data/SCBI_data_dictionary_2023_census.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herrmannV\Dropbox (Smithsonian)\GitHub\SCBI-ForestGEO\2023census\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/shuej_si_edu/Documents/Documents/GitHub/2023census/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25194A6-885B-4C01-9988-5DD7DA592AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="6_{966D63DF-4C50-42CD-9018-5613D1E3ACFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B850352-BB99-4F9D-9B0A-533D7209E576}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{BB1BC1A3-83C1-41A8-930A-6B2702BBB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="existing_trees" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">existing_trees!$B$1:$G$36</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="272">
   <si>
     <t>crown_position</t>
   </si>
@@ -845,6 +856,12 @@
   </si>
   <si>
     <t>no longer used</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Hollow stem</t>
   </si>
 </sst>
 </file>
@@ -1237,20 +1254,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CAB06-B581-49AF-A77A-B8530B1E5C50}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1282,7 +1299,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1296,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1325,7 +1342,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1348,7 +1365,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1368,7 +1385,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1391,7 +1408,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1405,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1419,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1442,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1456,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1476,7 +1493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1493,7 +1510,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1513,7 +1530,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1533,7 +1550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1553,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1570,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1596,7 +1613,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1619,7 +1636,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -1651,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1672,7 +1689,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1693,7 +1710,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1714,7 +1731,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1735,7 +1752,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1761,7 +1778,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1790,7 +1807,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1817,7 +1834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1840,7 +1857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1860,7 +1877,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1883,7 +1900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1901,7 +1918,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1925,19 +1942,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3688775-B1D1-40DD-BD64-506E041BD460}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1972,7 +1989,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1987,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2016,7 +2033,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2061,7 +2078,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2076,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2091,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2112,7 +2129,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2129,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2150,7 +2167,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2171,7 +2188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2195,7 +2212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2216,7 +2233,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2239,7 +2256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2272,7 +2289,7 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2301,7 +2318,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2327,7 +2344,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2351,7 +2368,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2372,7 +2389,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2396,7 +2413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -2413,7 +2430,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2430,7 +2447,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -2438,7 +2455,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2462,16 +2479,16 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -2503,7 +2520,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2526,7 +2543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2549,7 +2566,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2575,7 +2592,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2604,7 +2621,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2624,7 +2641,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2667,7 +2684,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2690,7 +2707,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2713,7 +2730,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2736,7 +2753,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2762,7 +2779,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2785,7 +2802,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2809,20 +2826,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550619-C900-43DA-89F1-CA09A5AF18CE}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>205</v>
       </c>
@@ -2839,7 +2856,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2850,7 +2867,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -2864,7 +2881,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2875,7 +2892,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -2886,7 +2903,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -2897,7 +2914,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -2908,7 +2925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2919,7 +2936,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2933,7 +2950,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -2944,7 +2961,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2955,7 +2972,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -2969,7 +2986,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -2980,7 +2997,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>125</v>
       </c>
@@ -2995,7 +3012,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>125</v>
       </c>
@@ -3010,7 +3027,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>125</v>
       </c>
@@ -3025,7 +3042,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>125</v>
       </c>
@@ -3040,7 +3057,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>125</v>
       </c>
@@ -3055,7 +3072,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>125</v>
       </c>
@@ -3070,7 +3087,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>125</v>
       </c>
@@ -3085,7 +3102,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -3096,7 +3113,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>113</v>
       </c>
@@ -3107,7 +3124,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3118,7 +3135,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3129,7 +3146,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3140,7 +3157,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3168,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +3179,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -3173,7 +3190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -3184,7 +3201,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3195,7 +3212,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>135</v>
       </c>
@@ -3206,7 +3223,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -3217,7 +3234,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -3228,7 +3245,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -3239,7 +3256,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3250,7 +3267,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -3261,7 +3278,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>135</v>
       </c>
@@ -3272,7 +3289,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>135</v>
       </c>
@@ -3283,7 +3300,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -3294,7 +3311,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -3305,7 +3322,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>135</v>
       </c>
@@ -3316,7 +3333,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -3327,7 +3344,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>135</v>
       </c>
@@ -3338,7 +3355,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>135</v>
       </c>
@@ -3349,7 +3366,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>135</v>
       </c>
@@ -3360,7 +3377,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -3371,179 +3388,190 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>270</v>
       </c>
       <c r="C47" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>4</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
         <v>3</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58">
         <v>3</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7</v>
       </c>
       <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61">
         <v>3</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3560,13 +3588,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3592,7 +3620,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3606,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3623,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3637,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -3651,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3665,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -3682,7 +3710,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -3699,7 +3727,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3716,7 +3744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -3736,7 +3764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -3754,7 +3782,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3771,7 +3799,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -3788,7 +3816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3809,7 +3837,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3826,7 +3854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -3843,7 +3871,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -3857,7 +3885,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3875,7 +3903,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -3896,7 +3924,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -3917,7 +3945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -3938,7 +3966,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -3957,7 +3985,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -3978,7 +4006,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -3999,7 +4027,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -4020,7 +4048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
@@ -4041,7 +4069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -4062,7 +4090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -4083,7 +4111,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -4104,7 +4132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
@@ -4136,12 +4164,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>144</v>
       </c>
@@ -4149,7 +4177,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -4157,7 +4185,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -4165,7 +4193,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -4173,7 +4201,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -4181,7 +4209,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -4189,7 +4217,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -4197,7 +4225,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -4205,7 +4233,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -4213,7 +4241,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -4237,9 +4265,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4247,7 +4275,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -4255,7 +4283,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -4263,7 +4291,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -4271,7 +4299,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -4279,7 +4307,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -4300,12 +4328,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4316,7 +4344,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4327,7 +4355,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4338,7 +4366,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4349,7 +4377,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>

</xml_diff>